<commit_message>
fix bugs with add TruckInfoService
</commit_message>
<xml_diff>
--- a/导入功能测试数据/超限超限信息导入.xlsx
+++ b/导入功能测试数据/超限超限信息导入.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="138">
   <si>
     <t>处罚觉定书编号</t>
   </si>
@@ -419,6 +419,17 @@
   </si>
   <si>
     <t>佛山超载超限</t>
+  </si>
+  <si>
+    <t>2月违规名单</t>
+  </si>
+  <si>
+    <t>粤BBL953</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄爱辉1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1400,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2969,6 +2980,41 @@
         <v>18</v>
       </c>
     </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A46" s="1">
+        <v>44019100045</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G46" s="2">
+        <v>42951</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I46" s="1">
+        <v>49.8</v>
+      </c>
+      <c r="J46" s="1">
+        <v>6</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- temp commit - TODO：更改ID生成规则
</commit_message>
<xml_diff>
--- a/导入功能测试数据/超限超限信息导入.xlsx
+++ b/导入功能测试数据/超限超限信息导入.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="183">
   <si>
     <t>处罚觉定书编号</t>
   </si>
@@ -430,6 +430,141 @@
   <si>
     <t>黄爱辉1</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2017082211010345</t>
+  </si>
+  <si>
+    <t>P2017082211010346</t>
+  </si>
+  <si>
+    <t>P2017082211010347</t>
+  </si>
+  <si>
+    <t>P2017082211010348</t>
+  </si>
+  <si>
+    <t>P2017082211010349</t>
+  </si>
+  <si>
+    <t>P2017082211010350</t>
+  </si>
+  <si>
+    <t>P2017082211010351</t>
+  </si>
+  <si>
+    <t>P2017082211010352</t>
+  </si>
+  <si>
+    <t>P2017082211010353</t>
+  </si>
+  <si>
+    <t>P2017082211010354</t>
+  </si>
+  <si>
+    <t>P2017082211010355</t>
+  </si>
+  <si>
+    <t>P2017082211010356</t>
+  </si>
+  <si>
+    <t>P2017082211010357</t>
+  </si>
+  <si>
+    <t>P2017082211010358</t>
+  </si>
+  <si>
+    <t>P2017082211010359</t>
+  </si>
+  <si>
+    <t>P2017082211010360</t>
+  </si>
+  <si>
+    <t>P2017082211010361</t>
+  </si>
+  <si>
+    <t>P2017082211010362</t>
+  </si>
+  <si>
+    <t>P2017082211010363</t>
+  </si>
+  <si>
+    <t>P2017082211010364</t>
+  </si>
+  <si>
+    <t>P2017082211010365</t>
+  </si>
+  <si>
+    <t>P2017082211010366</t>
+  </si>
+  <si>
+    <t>P2017082211010367</t>
+  </si>
+  <si>
+    <t>P2017082211010368</t>
+  </si>
+  <si>
+    <t>P2017082211010369</t>
+  </si>
+  <si>
+    <t>P2017082211010370</t>
+  </si>
+  <si>
+    <t>P2017082211010371</t>
+  </si>
+  <si>
+    <t>P2017082211010372</t>
+  </si>
+  <si>
+    <t>P2017082211010373</t>
+  </si>
+  <si>
+    <t>P2017082211010374</t>
+  </si>
+  <si>
+    <t>P2017082211010375</t>
+  </si>
+  <si>
+    <t>P2017082211010376</t>
+  </si>
+  <si>
+    <t>P2017082211010377</t>
+  </si>
+  <si>
+    <t>P2017082211010378</t>
+  </si>
+  <si>
+    <t>P2017082211010379</t>
+  </si>
+  <si>
+    <t>P2017082211010380</t>
+  </si>
+  <si>
+    <t>P2017082211010381</t>
+  </si>
+  <si>
+    <t>P2017082211010382</t>
+  </si>
+  <si>
+    <t>P2017082211010383</t>
+  </si>
+  <si>
+    <t>P2017082211010384</t>
+  </si>
+  <si>
+    <t>P2017082211010385</t>
+  </si>
+  <si>
+    <t>P2017082211010386</t>
+  </si>
+  <si>
+    <t>P2017082211010387</t>
+  </si>
+  <si>
+    <t>P2017082211010388</t>
+  </si>
+  <si>
+    <t>P2017082211010389</t>
   </si>
 </sst>
 </file>
@@ -1413,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1471,8 +1606,8 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
-        <v>44019100001</v>
+      <c r="A2" t="s">
+        <v>138</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -1506,8 +1641,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
-        <v>44019100002</v>
+      <c r="A3" t="s">
+        <v>139</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
@@ -1541,8 +1676,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
-        <v>44019100003</v>
+      <c r="A4" t="s">
+        <v>140</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>24</v>
@@ -1576,8 +1711,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A5" s="1">
-        <v>44019100004</v>
+      <c r="A5" t="s">
+        <v>141</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>27</v>
@@ -1614,8 +1749,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A6" s="1">
-        <v>44019100005</v>
+      <c r="A6" t="s">
+        <v>142</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>31</v>
@@ -1649,8 +1784,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
-        <v>44019100006</v>
+      <c r="A7" t="s">
+        <v>143</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>34</v>
@@ -1684,8 +1819,8 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
-        <v>44019100007</v>
+      <c r="A8" t="s">
+        <v>144</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>35</v>
@@ -1719,8 +1854,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A9" s="1">
-        <v>44019100008</v>
+      <c r="A9" t="s">
+        <v>145</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>36</v>
@@ -1751,8 +1886,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A10" s="1">
-        <v>44019100009</v>
+      <c r="A10" t="s">
+        <v>146</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>37</v>
@@ -1786,8 +1921,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A11" s="1">
-        <v>44019100010</v>
+      <c r="A11" t="s">
+        <v>147</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>38</v>
@@ -1821,8 +1956,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A12" s="1">
-        <v>44019100011</v>
+      <c r="A12" t="s">
+        <v>148</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>39</v>
@@ -1853,8 +1988,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A13" s="1">
-        <v>44019100012</v>
+      <c r="A13" t="s">
+        <v>149</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>40</v>
@@ -1888,8 +2023,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A14" s="1">
-        <v>44019100013</v>
+      <c r="A14" t="s">
+        <v>150</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>40</v>
@@ -1923,8 +2058,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A15" s="1">
-        <v>44019100014</v>
+      <c r="A15" t="s">
+        <v>151</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>40</v>
@@ -1955,8 +2090,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A16" s="1">
-        <v>44019100015</v>
+      <c r="A16" t="s">
+        <v>152</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>41</v>
@@ -1987,8 +2122,8 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A17" s="1">
-        <v>44019100016</v>
+      <c r="A17" t="s">
+        <v>153</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>42</v>
@@ -2022,8 +2157,8 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A18" s="1">
-        <v>44019100017</v>
+      <c r="A18" t="s">
+        <v>154</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>37</v>
@@ -2057,8 +2192,8 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A19" s="1">
-        <v>44019100018</v>
+      <c r="A19" t="s">
+        <v>155</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>38</v>
@@ -2092,8 +2227,8 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A20" s="1">
-        <v>44019100019</v>
+      <c r="A20" t="s">
+        <v>156</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>43</v>
@@ -2127,8 +2262,8 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A21" s="1">
-        <v>44019100020</v>
+      <c r="A21" t="s">
+        <v>157</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>44</v>
@@ -2162,8 +2297,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A22" s="1">
-        <v>44019100021</v>
+      <c r="A22" t="s">
+        <v>158</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>44</v>
@@ -2197,8 +2332,8 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A23" s="1">
-        <v>44019100022</v>
+      <c r="A23" t="s">
+        <v>159</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>40</v>
@@ -2232,8 +2367,8 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A24" s="1">
-        <v>44019100023</v>
+      <c r="A24" t="s">
+        <v>160</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>40</v>
@@ -2267,8 +2402,8 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A25" s="1">
-        <v>44019100024</v>
+      <c r="A25" t="s">
+        <v>161</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>44</v>
@@ -2299,8 +2434,8 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A26" s="1">
-        <v>44019100025</v>
+      <c r="A26" t="s">
+        <v>162</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>44</v>
@@ -2331,8 +2466,8 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A27" s="1">
-        <v>44019100026</v>
+      <c r="A27" t="s">
+        <v>163</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>45</v>
@@ -2363,8 +2498,8 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A28" s="1">
-        <v>44019100027</v>
+      <c r="A28" t="s">
+        <v>164</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>45</v>
@@ -2395,8 +2530,8 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A29" s="1">
-        <v>44019100028</v>
+      <c r="A29" t="s">
+        <v>165</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>46</v>
@@ -2427,8 +2562,8 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A30" s="1">
-        <v>44019100029</v>
+      <c r="A30" t="s">
+        <v>166</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>46</v>
@@ -2459,8 +2594,8 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A31" s="1">
-        <v>44019100030</v>
+      <c r="A31" t="s">
+        <v>167</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>47</v>
@@ -2491,8 +2626,8 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A32" s="1">
-        <v>44019100031</v>
+      <c r="A32" t="s">
+        <v>168</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>46</v>
@@ -2526,8 +2661,8 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A33" s="1">
-        <v>44019100032</v>
+      <c r="A33" t="s">
+        <v>169</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>47</v>
@@ -2561,8 +2696,8 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A34" s="1">
-        <v>44019100033</v>
+      <c r="A34" t="s">
+        <v>170</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>46</v>
@@ -2596,8 +2731,8 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A35" s="1">
-        <v>44019100034</v>
+      <c r="A35" t="s">
+        <v>171</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>47</v>
@@ -2631,8 +2766,8 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A36" s="1">
-        <v>44019100035</v>
+      <c r="A36" t="s">
+        <v>172</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>46</v>
@@ -2666,8 +2801,8 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A37" s="1">
-        <v>44019100036</v>
+      <c r="A37" t="s">
+        <v>173</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>47</v>
@@ -2701,8 +2836,8 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A38" s="1">
-        <v>44019100037</v>
+      <c r="A38" t="s">
+        <v>174</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>46</v>
@@ -2736,8 +2871,8 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A39" s="1">
-        <v>44019100038</v>
+      <c r="A39" t="s">
+        <v>175</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>47</v>
@@ -2771,8 +2906,8 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A40" s="1">
-        <v>44019100039</v>
+      <c r="A40" t="s">
+        <v>176</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>46</v>
@@ -2806,8 +2941,8 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A41" s="1">
-        <v>44019100040</v>
+      <c r="A41" t="s">
+        <v>177</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>47</v>
@@ -2841,8 +2976,8 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A42" s="1">
-        <v>44019100041</v>
+      <c r="A42" t="s">
+        <v>178</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>46</v>
@@ -2876,8 +3011,8 @@
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A43" s="1">
-        <v>44019100042</v>
+      <c r="A43" t="s">
+        <v>179</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>47</v>
@@ -2911,8 +3046,8 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A44" s="1">
-        <v>44019100043</v>
+      <c r="A44" t="s">
+        <v>180</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>46</v>
@@ -2946,8 +3081,8 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A45" s="1">
-        <v>44019100044</v>
+      <c r="A45" t="s">
+        <v>181</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>47</v>
@@ -2981,8 +3116,8 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A46" s="1">
-        <v>44019100045</v>
+      <c r="A46" t="s">
+        <v>182</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>47</v>

</xml_diff>